<commit_message>
Added program to loop over all files instead of just one file.
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -345,7 +345,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A3"/>
+  <dimension ref="A1:A5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -374,6 +374,20 @@
         </is>
       </c>
     </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>GETME</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>ALSOGETME</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>